<commit_message>
Prototypes: #3 Plugin for marking up code and viewing comments.
</commit_message>
<xml_diff>
--- a/eval/e19/tutorials.xlsx
+++ b/eval/e19/tutorials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="0" windowWidth="25600" windowHeight="25080" tabRatio="500"/>
+    <workbookView xWindow="6400" yWindow="0" windowWidth="28160" windowHeight="25080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>Link</t>
   </si>
@@ -179,13 +179,40 @@
   </si>
   <si>
     <t>Open Terminal, dt element, namespace, what is a soup, dictionary</t>
+  </si>
+  <si>
+    <t>RaspPi face det</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Face Recognition Using OpenCV</t>
+  </si>
+  <si>
+    <t>cv.CreateImage, OptionParser, cv.IPL_ORIGIN_TL, face.xml path</t>
+  </si>
+  <si>
+    <t>Raspberry Pi and the Camera Pi module: face recognition tutorial</t>
+  </si>
+  <si>
+    <t>terms: matrices, cascade, I2C, shield; open RaspPi terminal, WinSCP</t>
+  </si>
+  <si>
+    <t>Face Detection - Physical computing with Raspberry Pi</t>
+  </si>
+  <si>
+    <t>tuple assignment, drawRect args, why largest_blob is None</t>
+  </si>
+  <si>
+    <t>OpenCV Tutorial on Face Tracking - Raspberry PI Camera</t>
+  </si>
+  <si>
+    <t>with, format options, dtype=np.uint8, detectMultiscale args, CascadeClassifier silent fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -214,13 +241,6 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="16"/>
       <color theme="11"/>
       <name val="Calibri"/>
@@ -245,24 +265,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -593,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -639,19 +662,19 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -662,19 +685,19 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -685,19 +708,19 @@
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -708,19 +731,19 @@
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -731,19 +754,19 @@
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -754,19 +777,19 @@
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -777,19 +800,19 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -800,19 +823,19 @@
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -823,19 +846,19 @@
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -846,19 +869,19 @@
       <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -869,19 +892,19 @@
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -892,19 +915,19 @@
       <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -915,19 +938,19 @@
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -938,19 +961,19 @@
       <c r="B15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -961,19 +984,19 @@
       <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -981,22 +1004,22 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1004,7 +1027,7 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1021,6 +1044,98 @@
       </c>
       <c r="G18" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1042,6 +1157,10 @@
     <hyperlink ref="B16" r:id="rId15"/>
     <hyperlink ref="B17" r:id="rId16"/>
     <hyperlink ref="B18" r:id="rId17"/>
+    <hyperlink ref="B19" r:id="rId18"/>
+    <hyperlink ref="B20" r:id="rId19"/>
+    <hyperlink ref="B21" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Prototypes: #4 wget explanation generator.
</commit_message>
<xml_diff>
--- a/eval/e19/tutorials.xlsx
+++ b/eval/e19/tutorials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="0" windowWidth="28160" windowHeight="25080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
   <si>
     <t>Link</t>
   </si>
@@ -206,13 +206,37 @@
   </si>
   <si>
     <t>with, format options, dtype=np.uint8, detectMultiscale args, CascadeClassifier silent fail</t>
+  </si>
+  <si>
+    <t>wget</t>
+  </si>
+  <si>
+    <t>All the Wget Commands You Should Know</t>
+  </si>
+  <si>
+    <t>terms: mirror; number expansion {}, Terminal start, refer, cookies</t>
+  </si>
+  <si>
+    <t>Terminal scraping</t>
+  </si>
+  <si>
+    <t>Using the Linux Shell for Web Scraping</t>
+  </si>
+  <si>
+    <t>wget purpose, piping, -O -i options, CSS selector</t>
+  </si>
+  <si>
+    <t>Downloading an Entire Web Site with wget</t>
+  </si>
+  <si>
+    <t>Purpose of wget, where to run command, optimizations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -247,6 +271,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -274,11 +305,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -616,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1136,6 +1168,75 @@
       </c>
       <c r="G22" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1161,6 +1262,9 @@
     <hyperlink ref="B20" r:id="rId19"/>
     <hyperlink ref="B21" r:id="rId20"/>
     <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B23" r:id="rId22"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="B25" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Prototypes: #6, Java-based web server for NLG from JSON.
</commit_message>
<xml_diff>
--- a/eval/e19/tutorials.xlsx
+++ b/eval/e19/tutorials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="118">
   <si>
     <t>Link</t>
   </si>
@@ -229,7 +229,151 @@
     <t>Downloading an Entire Web Site with wget</t>
   </si>
   <si>
-    <t>Purpose of wget, where to run command, optimizations</t>
+    <t>Purpose of wget, where to run command, optimizations, line continuations</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>grun meaning, curl, export, executing Java path</t>
+  </si>
+  <si>
+    <t>Quick Start (Antlr)</t>
+  </si>
+  <si>
+    <t>Samples (Antlr)</t>
+  </si>
+  <si>
+    <t>Antlr quickstart</t>
+  </si>
+  <si>
+    <t>"grammar" purpose, RegEx, grun command, where to paste code</t>
+  </si>
+  <si>
+    <t>Antlr setup</t>
+  </si>
+  <si>
+    <t>Getting Started with ANTLR v4</t>
+  </si>
+  <si>
+    <t>Show Process</t>
+  </si>
+  <si>
+    <t>Save to /usr/local/lib on OSX, UNIX = OSX, adding to CLASSPATH, -Xmx500M, r command line opt</t>
+  </si>
+  <si>
+    <t>IntelliJ setup</t>
+  </si>
+  <si>
+    <t>Configuring Module Dependencies and Libraries</t>
+  </si>
+  <si>
+    <t>terms: module library, module dependencies, project structure</t>
+  </si>
+  <si>
+    <t>Antlr guide</t>
+  </si>
+  <si>
+    <t>Grammar Lexicon</t>
+  </si>
+  <si>
+    <t>Standards</t>
+  </si>
+  <si>
+    <t>terms: actions, Javadocs, Unicode, escape, reserved words</t>
+  </si>
+  <si>
+    <t>Grammar structure</t>
+  </si>
+  <si>
+    <t>terms: channels, lexer, parser, actions, depth-first search; | (or)</t>
+  </si>
+  <si>
+    <t>nginx HTTPS</t>
+  </si>
+  <si>
+    <t>How To Create an SSL Certificate on Nginx for Ubuntu 14.04</t>
+  </si>
+  <si>
+    <t>nginx 'listen 80', enable 443 only, Beast Attack, certificate authority</t>
+  </si>
+  <si>
+    <t>Java HTTP server</t>
+  </si>
+  <si>
+    <t>Hava a simple HTTP server</t>
+  </si>
+  <si>
+    <t>Java write JSON</t>
+  </si>
+  <si>
+    <t>JSON.Simple Example – Read And Write JSON</t>
+  </si>
+  <si>
+    <t>Introduction to the POM</t>
+  </si>
+  <si>
+    <t>maven, POM pieces: repository layout, url, updatePolicy, etc., FQAN</t>
+  </si>
+  <si>
+    <t>Maven Tutorial</t>
+  </si>
+  <si>
+    <t>Maven POM definition</t>
+  </si>
+  <si>
+    <t>proxy access, Eclipse IDE, web application, Tomcat</t>
+  </si>
+  <si>
+    <t>Teach (Fragment)</t>
+  </si>
+  <si>
+    <t>Maven build project</t>
+  </si>
+  <si>
+    <t>How To Build Project With Maven</t>
+  </si>
+  <si>
+    <t>maven, source location, install maven, war, packaging options</t>
+  </si>
+  <si>
+    <t>concept: JDK, HTTP server; throws Exception, InetSocketAddress, createContext, HttpHandler,  HttpExchange methods?, setExecutor, display PDF, naming class file</t>
+  </si>
+  <si>
+    <t>How To Create A Java Project With Maven</t>
+  </si>
+  <si>
+    <t>Maven run class</t>
+  </si>
+  <si>
+    <t>3 ways to run Java main from Maven</t>
+  </si>
+  <si>
+    <t>mvn installed, open Terminal, exec:java goal, maven phases, maven profiles, exec:java missing</t>
+  </si>
+  <si>
+    <t>{} means custom param, /src/ vs. src/, business logic, -cp, Eclipse IDE, example archetypes, non-empty dir init</t>
+  </si>
+  <si>
+    <t>terms: JSON; Maven setup, pom.xml, parse pure string how, where to insert pom dependency, what the rest says, empty JAR, including SRC, catch ParseException, local jars as deps</t>
+  </si>
+  <si>
+    <t>Maven local JAR</t>
+  </si>
+  <si>
+    <t>How to add local jar files in maven project?</t>
+  </si>
+  <si>
+    <t>Maven 3rd party JAR</t>
+  </si>
+  <si>
+    <t>Guide to installing 3rd party JARs</t>
+  </si>
+  <si>
+    <t>META-INF, pom file, group-id, artifact-id, packaging, location of local repo, include as dependency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Don't copy-paste all, example group-id, example artifact, path cannot include '~', </t>
   </si>
 </sst>
 </file>
@@ -296,7 +440,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -304,20 +448,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -648,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1237,6 +1386,371 @@
       </c>
       <c r="G25" s="1" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1265,6 +1779,22 @@
     <hyperlink ref="B23" r:id="rId22"/>
     <hyperlink ref="B24" r:id="rId23"/>
     <hyperlink ref="B25" r:id="rId24"/>
+    <hyperlink ref="B26" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="B40" r:id="rId39" location="answer-4955695"/>
+    <hyperlink ref="B41" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Evaluations: #19, updated tutorial list with tutorials from E26
</commit_message>
<xml_diff>
--- a/eval/e19/tutorials.xlsx
+++ b/eval/e19/tutorials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="25080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="168">
   <si>
     <t>Link</t>
   </si>
@@ -373,7 +373,157 @@
     <t>META-INF, pom file, group-id, artifact-id, packaging, location of local repo, include as dependency</t>
   </si>
   <si>
-    <t xml:space="preserve">Don't copy-paste all, example group-id, example artifact, path cannot include '~', </t>
+    <t>Don't copy-paste all, example group-id, example artifact, path cannot include '~', don't misspell 'jar'..., undo (uninstall)</t>
+  </si>
+  <si>
+    <t>Github API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET command, query parameters, curl -i, endpoints, </t>
+  </si>
+  <si>
+    <t>Getting Started</t>
+  </si>
+  <si>
+    <t>open command prompt, HTTP headers, Oauth model, create Github account, caching</t>
+  </si>
+  <si>
+    <t>Github Search API</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Reach</t>
+  </si>
+  <si>
+    <t>validation: specify user, org, or repo</t>
+  </si>
+  <si>
+    <t>requests_cache</t>
+  </si>
+  <si>
+    <t>requests-cache</t>
+  </si>
+  <si>
+    <t>terms: requests, headers; name of demo_cache, why errors avoided</t>
+  </si>
+  <si>
+    <t>requests_cache throttle</t>
+  </si>
+  <si>
+    <t>User guide</t>
+  </si>
+  <si>
+    <t>sqlite, mongodb, redis, expiration, transparent caching, CachedSession</t>
+  </si>
+  <si>
+    <t>SCP</t>
+  </si>
+  <si>
+    <t>SSH and SCP: Howto, tips &amp; tricks</t>
+  </si>
+  <si>
+    <t>open Terminal, different cmd prompt, server, how to backup</t>
+  </si>
+  <si>
+    <t>Python text processing</t>
+  </si>
+  <si>
+    <t>Python Recipe: Open a file, read it, print matching lines</t>
+  </si>
+  <si>
+    <t>open Terminal, why Python needed, what each command does, curl -O option, modifying RegEx</t>
+  </si>
+  <si>
+    <t>Python web scraping</t>
+  </si>
+  <si>
+    <t>Reading Data from the Web: Web Scraping &amp; Regular Expressions</t>
+  </si>
+  <si>
+    <t>import, '.' in import path, what decode() does, index, !=, list slicing, HTTP GET and POST</t>
+  </si>
+  <si>
+    <t>Beautiful Soup 4 Python</t>
+  </si>
+  <si>
+    <t>Beautiful Soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apt-get, urllib2 for fetching URLs, filter concept, iterate over function return, print(), </t>
+  </si>
+  <si>
+    <t>Python Log Analysis</t>
+  </si>
+  <si>
+    <t>Log file analysis - short Python example</t>
+  </si>
+  <si>
+    <t>Demonstrate</t>
+  </si>
+  <si>
+    <t>inline dict declaration, os.listdir("."), "ac" prefix, xreadlines, .get(a, b), continue, string concat, .__cmp__, pass func as argument, -1 index, instance variables, slicing, RegEx</t>
+  </si>
+  <si>
+    <t>Python text mining</t>
+  </si>
+  <si>
+    <t>An Introduction to Text Mining using Twitter Streaming API and Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">term:keyword, term:access token, from-import, class, install pandas and matplotlib, import-as, UNIX paths, map, RegEx, .value_counts, list comprehension, index by relation, </t>
+  </si>
+  <si>
+    <t>Python programming - text and web mining</t>
+  </si>
+  <si>
+    <t>can_fetch args, viewing Apache log, urllib opener, term:user-agent, JSON, dict.update, try-except, term:status codes, time.time(), list comprehension, hold(), enumerate, solid_capstyle='butt', hist, formatter.NullFormatter, p.anchorlist, nltk installation, BeautifulSoup installation, text=True, slicing, processes, zip, pool.map, line continuation, term:feeds, regular expressions, triple-quote strings, node name and value, join, term: template engine, {{ }} Jinja2 syntax, term: part of speech, pos_tag, tuple assignment, tuple iteration, slice, concept:grammar, cp.parse, lambda, hasattr, recursion, set, urlparse vs. urlunparse, negative indexes, scrapy installation, dot in import path, SgmlLinkExtractor(), callback, XPath, mod operator, extend, GetNextLink, term:MediaWiki, Brede Database, siblings, dict(**kwargs), range, FreqDist, random.shuffle, naive Bayes classifier,</t>
+  </si>
+  <si>
+    <t>Mining Twitter Data with Python</t>
+  </si>
+  <si>
+    <t>open 'r' option, indent=4, concept: tweet data, concept:overflow, install nltk,</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Python text validation</t>
+  </si>
+  <si>
+    <t>Python text validation: a-z and comma ","</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set, list comprehension, concept: timeit, all, None, re.compile, isalpha, list comprehension, RegEx, concept:ASCII indexes, ord, </t>
+  </si>
+  <si>
+    <t>Cerberus GSG</t>
+  </si>
+  <si>
+    <t>Welcome to Cerberus</t>
+  </si>
+  <si>
+    <t>concept: validation, concept: error types, SchemaError, python dictionary, ValidationError, error: unbalanced quotes, class definition, style: _ function name, &amp;, bool(), BSON, concept:nullable, concept:dependency</t>
+  </si>
+  <si>
+    <t>Form validation</t>
+  </si>
+  <si>
+    <t>Form and field validation | Django documentation | Django</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concept: method, is_valid, full_clean, Field, concept:normalizing, _, kwargs, format syntax, term:slug, RegEx, Django Field declaration, super, </t>
+  </si>
+  <si>
+    <t>Bottle App dev</t>
+  </si>
+  <si>
+    <t>Tutorial: Todo-List Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concept: WSGI, SQLite, localhost, mod_wsgi, decorators, easy_install, install SQLite, port number, from-import, cursor, </t>
   </si>
 </sst>
 </file>
@@ -797,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1751,6 +1901,397 @@
       </c>
       <c r="G41" s="1" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1795,6 +2336,23 @@
     <hyperlink ref="B39" r:id="rId38"/>
     <hyperlink ref="B40" r:id="rId39" location="answer-4955695"/>
     <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45" location="usage"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="B58" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Evaluations: #19, #26, cleanup and store new data
</commit_message>
<xml_diff>
--- a/eval/e19/tutorials.xlsx
+++ b/eval/e19/tutorials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="184">
   <si>
     <t>Link</t>
   </si>
@@ -524,13 +524,61 @@
   </si>
   <si>
     <t xml:space="preserve">concept: WSGI, SQLite, localhost, mod_wsgi, decorators, easy_install, install SQLite, port number, from-import, cursor, </t>
+  </si>
+  <si>
+    <t>Web hover popups</t>
+  </si>
+  <si>
+    <t>Wickham's HTML &amp; CSS Tutorial</t>
+  </si>
+  <si>
+    <t>npm bookmarklet compilation</t>
+  </si>
+  <si>
+    <t>bookmarklet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concept:bookmarklet, uglify-js, noConflict, concept:script includes, </t>
+  </si>
+  <si>
+    <t>javallone/regexper</t>
+  </si>
+  <si>
+    <t>RegExper Coding GSG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gulp, npm, bundle, </t>
+  </si>
+  <si>
+    <t>Gulp error resolution</t>
+  </si>
+  <si>
+    <t>Gulp error with gulp-compass : You must compile individual stylesheets from the project directory</t>
+  </si>
+  <si>
+    <t>Error Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gulp purpose, term:sass, term:compass watch, gulpfile.js, plumber(), package.json, config.rb, </t>
+  </si>
+  <si>
+    <t>Yeoman bookmarklet</t>
+  </si>
+  <si>
+    <t>passy/generator-bookmarklet</t>
+  </si>
+  <si>
+    <t>Yeoman, app/ directory, dist/ folder, npm, -g</t>
+  </si>
+  <si>
+    <t>term: IE, concept:stylesheet, span, .php extension, br, alt, CSS selectors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -565,13 +613,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -590,7 +631,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -600,16 +641,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -617,6 +658,8 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -947,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1473,7 +1516,7 @@
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1496,7 +1539,7 @@
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1519,7 +1562,7 @@
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1703,7 +1746,7 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1726,7 +1769,7 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1749,7 +1792,7 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1772,7 +1815,7 @@
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1795,7 +1838,7 @@
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1818,7 +1861,7 @@
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1841,7 +1884,7 @@
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1864,7 +1907,7 @@
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1884,7 +1927,7 @@
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1907,7 +1950,7 @@
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1930,7 +1973,7 @@
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1953,7 +1996,7 @@
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1976,7 +2019,7 @@
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1999,7 +2042,7 @@
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2022,7 +2065,7 @@
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2045,7 +2088,7 @@
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -2068,7 +2111,7 @@
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -2091,7 +2134,7 @@
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2114,7 +2157,7 @@
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2137,7 +2180,7 @@
       <c r="A52" s="1">
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2160,7 +2203,7 @@
       <c r="A53" s="1">
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -2183,7 +2226,7 @@
       <c r="A54" s="1">
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2206,7 +2249,7 @@
       <c r="A55" s="1">
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -2229,7 +2272,7 @@
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2252,7 +2295,7 @@
       <c r="A57" s="1">
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -2275,7 +2318,7 @@
       <c r="A58" s="1">
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -2292,6 +2335,121 @@
       </c>
       <c r="G58" s="1" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2353,6 +2511,11 @@
     <hyperlink ref="B56" r:id="rId55"/>
     <hyperlink ref="B57" r:id="rId56"/>
     <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B63" r:id="rId62"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>